<commit_message>
Changed groups to be created by default
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4631039B-7194-490B-8D96-5CC11F0C1FFD}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{821393D9-0589-4F84-B1F3-6867FD07D47A}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -741,7 +743,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -796,7 +798,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -825,7 +827,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -854,7 +856,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -883,7 +885,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -912,7 +914,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -941,7 +943,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -970,7 +972,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -999,7 +1001,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -1241,21 +1243,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -1439,10 +1426,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1464,19 +1476,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lot more intune stuff, stick creation, language pack fixes, local printer fixes, aip enhancements and lot more
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37067CFD-45A3-4238-9D55-CA40C4AD59BB}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E029D66D-8D97-4F33-833B-5BA3D2A81C71}"/>
   <bookViews>
-    <workbookView xWindow="2226" yWindow="420" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="528" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
   <si>
     <t>Type</t>
   </si>
@@ -48,9 +48,6 @@
     <t>DanymicRule</t>
   </si>
   <si>
-    <t>WelcomeMessageEnabled</t>
-  </si>
-  <si>
     <t>MFA is disabled for members in this group</t>
   </si>
   <si>
@@ -69,18 +66,6 @@
     <t>(user.userType -eq "Guest")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-MFADISABLED</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-O365GROUPMANAGERS</t>
-  </si>
-  <si>
-    <t>ALYAOG-ADM-AlleExternen</t>
-  </si>
-  <si>
-    <t>ALYAOG-ADM-AlleInternen</t>
-  </si>
-  <si>
     <t>(user.userType -eq "User")</t>
   </si>
   <si>
@@ -97,6 +82,174 @@
   </si>
   <si>
     <t>Licenses</t>
+  </si>
+  <si>
+    <t>O365GrpHiddenFromAddressListsEnabled</t>
+  </si>
+  <si>
+    <t>O365GrpCalendarMemberReadOnly</t>
+  </si>
+  <si>
+    <t>O365GrpRejectMessagesFromSendersOrMembers</t>
+  </si>
+  <si>
+    <t>O365GrpUnifiedGroupWelcomeMessageEnabled</t>
+  </si>
+  <si>
+    <t>O365GrpSubscriptionEnabled</t>
+  </si>
+  <si>
+    <t>O365GrpModerationEnabled</t>
+  </si>
+  <si>
+    <t>O365GrpHiddenFromExchangeClientsEnabled</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>MFA is enabled for members in this group</t>
+  </si>
+  <si>
+    <t>Members of this group can register devices</t>
+  </si>
+  <si>
+    <t>Holds all devices with a standard configuration</t>
+  </si>
+  <si>
+    <t>(device.deviceCategory -eq "Standard")</t>
+  </si>
+  <si>
+    <t>Holds all autopilot devices</t>
+  </si>
+  <si>
+    <t>(device.devicePhysicalIDs -any (_ -contains "[ZTDId]"))</t>
+  </si>
+  <si>
+    <t>Holds all standard autopilot devices</t>
+  </si>
+  <si>
+    <t>(device.devicePhysicalIds -any (_ -eq "[OrderID]:Standard"))</t>
+  </si>
+  <si>
+    <t>Used to configure licenses</t>
+  </si>
+  <si>
+    <t>SPE_E3</t>
+  </si>
+  <si>
+    <t>STANDARDPACK</t>
+  </si>
+  <si>
+    <t>EXCHANGEDESKLESS</t>
+  </si>
+  <si>
+    <t>POWER_BI_STANDARD</t>
+  </si>
+  <si>
+    <t>O365_BUSINESS_ESSENTIALS</t>
+  </si>
+  <si>
+    <t>FLOW_FREE</t>
+  </si>
+  <si>
+    <t>SMB_APPS</t>
+  </si>
+  <si>
+    <t>SHAREPOINTSTANDARD</t>
+  </si>
+  <si>
+    <t>MCOCAP</t>
+  </si>
+  <si>
+    <t>PHONESYSTEM_VIRTUALUSER</t>
+  </si>
+  <si>
+    <t>Members of this group get specified apps asigned in WVD test</t>
+  </si>
+  <si>
+    <t>Members of this group get specified apps asigned</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-MFADISABLED</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-MFAENABLED</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-O365GROUPMANAGERS</t>
+  </si>
+  <si>
+    <t>XXXXOG-ADM-AlleInternen</t>
+  </si>
+  <si>
+    <t>XXXXOG-ADM-AlleExternen</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEADMINS</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICESTANDARD</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEAUTOPILOT</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEAUTOPILOTSTANDARD</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICMS365E3FULL</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICO365E1FULL</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICEXCHKIOSK</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICPBIFREE</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICMS365BUSBASIC</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICFLOWFREE</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICSMBAPPS</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICSPP1</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICCOMMPHONE</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICVIRTPHONE</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPTDSKTP</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPTSTD</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPTVISIO</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPTPRJCT</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPDSKTP</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPSTD</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPVISIO</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-APPPRJCT</t>
   </si>
 </sst>
 </file>
@@ -147,7 +300,50 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -481,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -495,12 +691,11 @@
     <col min="7" max="7" width="8.83984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49.68359375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -524,129 +719,775 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
       <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
         <v>0</v>
       </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:P1048576">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:P3">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF(OR($B3="O365Group",$B3="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:P10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(OR($B9="O365Group",$B9="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -830,35 +1671,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -880,9 +1696,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added scripts for dns migration and a SharePoint user access export
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E029D66D-8D97-4F33-833B-5BA3D2A81C71}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75AA26AF-1F6E-4635-9F38-A6C1E5523B8E}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="528" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="102">
   <si>
     <t>Type</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Used to configure licenses</t>
   </si>
   <si>
-    <t>SPE_E3</t>
-  </si>
-  <si>
     <t>STANDARDPACK</t>
   </si>
   <si>
@@ -147,24 +144,9 @@
     <t>POWER_BI_STANDARD</t>
   </si>
   <si>
-    <t>O365_BUSINESS_ESSENTIALS</t>
-  </si>
-  <si>
     <t>FLOW_FREE</t>
   </si>
   <si>
-    <t>SMB_APPS</t>
-  </si>
-  <si>
-    <t>SHAREPOINTSTANDARD</t>
-  </si>
-  <si>
-    <t>MCOCAP</t>
-  </si>
-  <si>
-    <t>PHONESYSTEM_VIRTUALUSER</t>
-  </si>
-  <si>
     <t>Members of this group get specified apps asigned in WVD test</t>
   </si>
   <si>
@@ -198,36 +180,6 @@
     <t>XXXXSG-ADM-DEVICEAUTOPILOTSTANDARD</t>
   </si>
   <si>
-    <t>XXXXSG-ADM-LICMS365E3FULL</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICO365E1FULL</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICEXCHKIOSK</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICPBIFREE</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICMS365BUSBASIC</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICFLOWFREE</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICSMBAPPS</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICSPP1</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICCOMMPHONE</t>
-  </si>
-  <si>
-    <t>XXXXSG-ADM-LICVIRTPHONE</t>
-  </si>
-  <si>
     <t>XXXXSG-ADM-APPTDSKTP</t>
   </si>
   <si>
@@ -250,6 +202,135 @@
   </si>
   <si>
     <t>XXXXSG-ADM-APPPRJCT</t>
+  </si>
+  <si>
+    <t>Holds all mac devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "MacMDM")</t>
+  </si>
+  <si>
+    <t>Holds all mac company owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "MacMDM") -and (device.deviceOwnership -eq "Company")</t>
+  </si>
+  <si>
+    <t>Holds all mac personal owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "MacMDM") -and (device.deviceOwnership -ne "Company")</t>
+  </si>
+  <si>
+    <t>Holds all android devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "Android")</t>
+  </si>
+  <si>
+    <t>Holds all android company owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "Android") -and (device.deviceOwnership -eq "Company")</t>
+  </si>
+  <si>
+    <t>Holds all android personal owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "Android") -and (device.deviceOwnership -ne "Company")</t>
+  </si>
+  <si>
+    <t>Holds all ios devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone")</t>
+  </si>
+  <si>
+    <t>Holds all ios company owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.deviceOwnership -eq "Company")</t>
+  </si>
+  <si>
+    <t>Holds all ios personal owned devices</t>
+  </si>
+  <si>
+    <t>(device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.deviceOwnership -ne "Company")</t>
+  </si>
+  <si>
+    <t>O365_BUSINESS_PREMIUM</t>
+  </si>
+  <si>
+    <t>SPE_E5</t>
+  </si>
+  <si>
+    <t>VISIOCLIENT</t>
+  </si>
+  <si>
+    <t>DYN365_ENTERPRISE_P1_IW</t>
+  </si>
+  <si>
+    <t>Dynamics_365_Onboarding_SKU</t>
+  </si>
+  <si>
+    <t>POWER_BI_PRO</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEMAC</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEMACOWNED</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEMACPERSONAL</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEANDROID</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEANDROIDOWNED</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEANDROIDPERSONAL</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEIOS</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEIOSOWNED</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-DEVICEIOSPERSONAL</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICMS365BusinessStdFull</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICMS365E5Full</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICO365E1Full</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICVisio</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICFlowFree</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICD365EntP1Trial</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICD365OnboardingTrial</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICPowerBIFree</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICPowerBIPro</t>
+  </si>
+  <si>
+    <t>XXXXSG-ADM-LICExchangeKiosk</t>
   </si>
 </sst>
 </file>
@@ -300,7 +381,49 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -677,7 +800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -751,16 +874,16 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -774,16 +897,16 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -797,16 +920,16 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -820,16 +943,16 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -867,16 +990,16 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -908,25 +1031,28 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -937,22 +1063,22 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -963,22 +1089,22 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -989,22 +1115,22 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1015,22 +1141,22 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
-      <c r="I11" t="s">
-        <v>36</v>
+      <c r="H11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1041,22 +1167,22 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
-        <v>37</v>
+      <c r="H12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1067,22 +1193,22 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" t="s">
-        <v>38</v>
+      <c r="H13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1093,22 +1219,22 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" t="s">
-        <v>39</v>
+      <c r="H14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1119,22 +1245,22 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
       </c>
-      <c r="I15" t="s">
-        <v>40</v>
+      <c r="H15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1145,22 +1271,22 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
       </c>
-      <c r="I16" t="s">
-        <v>41</v>
+      <c r="H16" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1171,22 +1297,19 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
-      </c>
-      <c r="I17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1197,22 +1320,22 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="I18" t="s">
-        <v>43</v>
+      <c r="H18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1223,22 +1346,22 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="I19" t="s">
-        <v>44</v>
+      <c r="H19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1249,22 +1372,22 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
       </c>
       <c r="I20" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1275,19 +1398,22 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1298,19 +1424,22 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1321,19 +1450,22 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1344,19 +1476,22 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1367,19 +1502,22 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1390,19 +1528,22 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1413,19 +1554,22 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1436,35 +1580,288 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
       </c>
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J1:P1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="J1:P6 J38:P1048576">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:P3">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>IF(OR($B3="O365Group",$B3="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:P10">
+  <conditionalFormatting sqref="J7:P7 J11:P11 J17:P37">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>IF(OR($B7="O365Group",$B7="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:P12">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>IF(OR($B12="O365Group",$B12="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:P8">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>IF(OR($B8="O365Group",$B8="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:P9">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>IF(OR($B9="O365Group",$B9="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:P14">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>IF(OR($B14="O365Group",$B14="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:P15">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>IF(OR($B15="O365Group",$B15="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:P10">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF(OR($B10="O365Group",$B10="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:P13">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF(OR($B13="O365Group",$B13="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:P16">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(OR($B9="O365Group",$B9="Type"),faslch,TRUE)</formula>
+      <formula>IF(OR($B16="O365Group",$B16="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1482,12 +1879,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -1671,6 +2062,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>
@@ -1680,22 +2077,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18209EA7-04F6-445D-8F30-F19FC7D76916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e7596eec-0011-44fa-9047-92dcd650b5d7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1711,4 +2092,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18209EA7-04F6-445D-8F30-F19FC7D76916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e7596eec-0011-44fa-9047-92dcd650b5d7"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed AD login to token based from az login
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75AA26AF-1F6E-4635-9F38-A6C1E5523B8E}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{D16535C0-5386-409B-B31B-BE7B156E7CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5AE5E61-C5FA-481C-A334-23F900FE2C02}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>(user.userType -eq "Guest")</t>
   </si>
   <si>
-    <t>(user.userType -eq "User")</t>
-  </si>
-  <si>
     <t>SecurityGroup</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>XXXXSG-ADM-LICExchangeKiosk</t>
+  </si>
+  <si>
+    <t>(user.userType -eq "Member")</t>
   </si>
 </sst>
 </file>
@@ -381,14 +381,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -818,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -842,48 +835,48 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -891,22 +884,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -914,22 +907,22 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -937,28 +930,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -984,22 +977,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -1031,282 +1024,282 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
         <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
         <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
         <v>63</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
         <v>65</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
         <v>67</v>
-      </c>
-      <c r="F12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
         <v>71</v>
-      </c>
-      <c r="F14" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
         <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
         <v>75</v>
-      </c>
-      <c r="F16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1314,334 +1307,334 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
         <v>31</v>
-      </c>
-      <c r="F18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
         <v>33</v>
-      </c>
-      <c r="F19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
       </c>
       <c r="I20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
         <v>35</v>
-      </c>
-      <c r="F22" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
       </c>
       <c r="I23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
       </c>
       <c r="I25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
       </c>
       <c r="I26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
         <v>8</v>
@@ -1649,22 +1642,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
         <v>8</v>
@@ -1672,22 +1665,22 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
@@ -1695,22 +1688,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
         <v>8</v>
@@ -1718,22 +1711,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
@@ -1741,22 +1734,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
         <v>8</v>
@@ -1764,22 +1757,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
@@ -1787,22 +1780,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -1810,12 +1803,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:P6 J38:P1048576">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:P3">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>IF(OR($B3="O365Group",$B3="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1870,15 +1863,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -2062,6 +2046,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2069,14 +2062,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2090,6 +2075,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Some fixes and merges from customer repos
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC611CFA-295A-4728-ABFB-574074160EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AC611CFA-295A-4728-ABFB-574074160EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{971CFC8F-FD81-43F6-9659-706A43D2720F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1260" windowWidth="22668" windowHeight="11808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="155">
   <si>
     <t>Type</t>
   </si>
@@ -192,322 +192,304 @@
     <t>ALYAOG-ADM-AlleExternen</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEADMINS</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICESTANDARD</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEAUTOPILOT</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEAUTOPILOTSTANDARD</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEMACALL</t>
-  </si>
-  <si>
     <t>(device.deviceOSType -match "Mac")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEMACMDM</t>
-  </si>
-  <si>
     <t>Holds all mdm mac devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Mac") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEMACMDMOWNED</t>
-  </si>
-  <si>
     <t>Holds all mdm mac company owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Mac") -and (device.deviceOwnership -eq "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEMACMDMPERSONAL</t>
-  </si>
-  <si>
     <t>Holds all mdm mac personal owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Mac") -and (device.deviceOwnership -ne "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEMACADE</t>
-  </si>
-  <si>
     <t>Holds all ade mac devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Mac") -and (device.enrollmentProfileName -eq "ALYA-MAC-ADE-Profile")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDALL</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEANDROIDALLSAMSUNG</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEANDROIDSAMSUNG</t>
-  </si>
-  <si>
     <t>Holds all android Samsung devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceManufacturer -eq "samsung")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDALLBLACKBERRY</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEANDROIDBLACKBERRY</t>
-  </si>
-  <si>
     <t>Holds all android BlackBerry devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceManufacturer -eq "BlackBerry")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDALLGOOGLE</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEANDROIDGOOGLE</t>
-  </si>
-  <si>
     <t>Holds all android Google devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceManufacturer -eq "Google")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDALLONEPLUS</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-DEVICEANDROIDONEPLUS</t>
-  </si>
-  <si>
     <t>Holds all android OnePlus devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceManufacturer -eq "OnePlus")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDMDM</t>
-  </si>
-  <si>
     <t>Holds all mdm android devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDMDMOWNED</t>
-  </si>
-  <si>
     <t>Holds all mdm android company owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceOwnership -eq "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEANDROIDMDMPERSONAL</t>
-  </si>
-  <si>
     <t>Holds all mdm android personal owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "Android") -and (device.deviceOwnership -ne "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEIOSALL</t>
-  </si>
-  <si>
     <t>(device.deviceOSType -match "iOs" -or device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEIOSMDM</t>
-  </si>
-  <si>
     <t>Holds all mdm ios devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "iOs" -or device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEIOSMDMOWNED</t>
-  </si>
-  <si>
     <t>Holds all mdm ios company owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "iOs" -or device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.deviceOwnership -eq "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEIOSMDMPERSONAL</t>
-  </si>
-  <si>
     <t>Holds all mdm ios personal owned devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "iOs" -or device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.deviceOwnership -ne "Company") -and (device.managementType -eq "MDM")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-DEVICEIOSADE</t>
-  </si>
-  <si>
     <t>Holds all ade ios devices</t>
   </si>
   <si>
     <t>(device.deviceOSType -match "iOs" -or device.deviceOSType -match "iPad" -or device.deviceOSType -match "iPhone") -and (device.enrollmentProfileName -eq "ALYA-iOS-ADE-Profile")</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICAADBASIC</t>
-  </si>
-  <si>
     <t>AAD_BASIC</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICAADP2</t>
-  </si>
-  <si>
     <t>AAD_PREMIUM_P2</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICCOMMPHONE</t>
-  </si>
-  <si>
     <t>MCOCAP</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICDYN365P1</t>
-  </si>
-  <si>
     <t>DYN365_ENTERPRISE_PLAN1</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICEMS</t>
-  </si>
-  <si>
     <t>EMS</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICEXCHKIOSK</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICEXCHP1</t>
-  </si>
-  <si>
     <t>EXCHANGESTANDARD</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICFLOWFREE</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICINTUNE</t>
-  </si>
-  <si>
     <t>INTUNE_A</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICMS365BUSBASICFULL</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICMS365BUSBASIC</t>
-  </si>
-  <si>
     <t>O365_BUSINESS_ESSENTIALS</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICMS365BUSSTDFULL</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICMS365BusinessStdFull</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICMS365E3FULL</t>
-  </si>
-  <si>
     <t>SPE_E3</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICMS365E5FULL</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICMS365E5Full</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICO365E1FULL</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICO365E3FULL</t>
-  </si>
-  <si>
     <t>ENTERPRISEPACK</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICPBIFREE</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICPBIPRO</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICPowerBIPro</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICSMBAPPS</t>
-  </si>
-  <si>
     <t>SMB_APPS</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICSPP1</t>
-  </si>
-  <si>
     <t>SHAREPOINTSTANDARD</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICVIRTPHONE</t>
-  </si>
-  <si>
     <t>PHONESYSTEM_VIRTUALUSER</t>
   </si>
   <si>
-    <t>ALYASG-ADM-LICVISIO2</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-LICVIVATOP</t>
-  </si>
-  <si>
     <t>TOPIC_EXPERIENCES</t>
   </si>
   <si>
-    <t>ALYASG-ADM-APPTDSKTP</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPTSTD</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPTVISIO</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPTPRJCT</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPDSKTP</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPSTD</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPVISIO</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-APPPRJCT</t>
+    <t>ALYASG-DEV-ADMINS</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-STANDARD</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-AUTOPILOT</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-AUTOPILOTSTANDARD</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-MACALL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-MACMDM</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-MACMDMOWNED</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-MACMDMPERSONAL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-MACADE</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDALL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDALLSAMSUNG</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDALLBLACKBERRY</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDALLGOOGLE</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDALLONEPLUS</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDMDM</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDMDMOWNED</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-ANDROIDMDMPERSONAL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-IOSALL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-IOSMDM</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-IOSMDMOWNED</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-IOSMDMPERSONAL</t>
+  </si>
+  <si>
+    <t>ALYASG-DEV-IOSADE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-AADBASIC</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-AADP2</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-COMMPHONE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365P1</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EMS</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EXCHKIOSK</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EXCHP1</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-FLOWFREE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-INTUNE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSBASICFULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSSTDFULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365E3FULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365E5FULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-O365E1FULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-O365E3FULL</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PBIFREE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PBIPRO</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-SMBAPPS</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-SPP1</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-VIRTPHONE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-VISIO2</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-VIVATOP</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-TDSKTP</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-TSTD</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-TVISIO</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-TPRJCT</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-DSKTP</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-STD</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-VISIO</t>
+  </si>
+  <si>
+    <t>ALYASG-APP-PRJCT</t>
+  </si>
+  <si>
+    <t>SPB</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSPREMFULL</t>
   </si>
 </sst>
 </file>
@@ -579,77 +561,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1040,24 +952,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1015625" customWidth="1"/>
-    <col min="4" max="4" width="11.26171875" customWidth="1"/>
-    <col min="5" max="5" width="26.5234375" customWidth="1"/>
-    <col min="6" max="6" width="31.5234375" customWidth="1"/>
-    <col min="7" max="7" width="7.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.7890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1107,7 +1019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1148,7 +1060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1169,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1263,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1271,10 +1183,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
@@ -1283,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1291,10 +1203,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -1306,7 +1218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1314,10 +1226,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -1329,7 +1241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1337,10 +1249,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>32</v>
@@ -1352,7 +1264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1360,10 +1272,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>41</v>
@@ -1372,102 +1284,102 @@
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="G14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1475,10 +1387,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>42</v>
@@ -1490,7 +1402,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1498,160 +1410,160 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="2" t="s">
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="G23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1659,10 +1571,10 @@
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>44</v>
@@ -1671,10 +1583,10 @@
         <v>8</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1682,22 +1594,22 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1705,22 +1617,22 @@
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1728,22 +1640,22 @@
         <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1751,22 +1663,22 @@
         <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -1774,10 +1686,10 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>34</v>
@@ -1786,10 +1698,10 @@
         <v>8</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
@@ -1797,10 +1709,10 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>34</v>
@@ -1809,10 +1721,10 @@
         <v>8</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -1820,10 +1732,10 @@
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>34</v>
@@ -1832,10 +1744,10 @@
         <v>8</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>25</v>
       </c>
@@ -1843,10 +1755,10 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>34</v>
@@ -1855,10 +1767,10 @@
         <v>8</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -1866,10 +1778,10 @@
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>34</v>
@@ -1878,10 +1790,10 @@
         <v>8</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -1889,10 +1801,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>34</v>
@@ -1904,7 +1816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>25</v>
       </c>
@@ -1912,10 +1824,10 @@
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>34</v>
@@ -1924,10 +1836,10 @@
         <v>8</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -1935,10 +1847,10 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>34</v>
@@ -1950,7 +1862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
@@ -1958,10 +1870,10 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>34</v>
@@ -1970,10 +1882,10 @@
         <v>8</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>25</v>
       </c>
@@ -1981,10 +1893,10 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>34</v>
@@ -1993,10 +1905,10 @@
         <v>8</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>25</v>
       </c>
@@ -2004,7 +1916,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>133</v>
@@ -2019,7 +1931,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>25</v>
       </c>
@@ -2027,10 +1939,10 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>34</v>
@@ -2039,10 +1951,10 @@
         <v>8</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>25</v>
       </c>
@@ -2050,10 +1962,10 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>34</v>
@@ -2062,10 +1974,10 @@
         <v>8</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>25</v>
       </c>
@@ -2073,10 +1985,10 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>34</v>
@@ -2085,10 +1997,10 @@
         <v>8</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>25</v>
       </c>
@@ -2096,10 +2008,10 @@
         <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>34</v>
@@ -2108,10 +2020,10 @@
         <v>8</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
@@ -2119,10 +2031,10 @@
         <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>34</v>
@@ -2131,10 +2043,10 @@
         <v>8</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>25</v>
       </c>
@@ -2142,10 +2054,10 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>34</v>
@@ -2154,10 +2066,10 @@
         <v>8</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>25</v>
       </c>
@@ -2165,10 +2077,10 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>34</v>
@@ -2177,10 +2089,10 @@
         <v>8</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
@@ -2188,10 +2100,10 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>34</v>
@@ -2200,10 +2112,10 @@
         <v>8</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>25</v>
       </c>
@@ -2211,10 +2123,10 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>34</v>
@@ -2223,10 +2135,10 @@
         <v>8</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>25</v>
       </c>
@@ -2234,10 +2146,10 @@
         <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>34</v>
@@ -2246,10 +2158,10 @@
         <v>8</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
@@ -2257,10 +2169,10 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>34</v>
@@ -2269,30 +2181,33 @@
         <v>8</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>25</v>
       </c>
@@ -2300,10 +2215,10 @@
         <v>13</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>39</v>
@@ -2312,7 +2227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>25</v>
       </c>
@@ -2320,10 +2235,10 @@
         <v>13</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>39</v>
@@ -2332,7 +2247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>25</v>
       </c>
@@ -2340,10 +2255,10 @@
         <v>13</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>39</v>
@@ -2352,7 +2267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>25</v>
       </c>
@@ -2360,19 +2275,19 @@
         <v>13</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>25</v>
       </c>
@@ -2380,10 +2295,10 @@
         <v>13</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>40</v>
@@ -2392,7 +2307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>25</v>
       </c>
@@ -2400,10 +2315,10 @@
         <v>13</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>40</v>
@@ -2412,7 +2327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>25</v>
       </c>
@@ -2420,10 +2335,10 @@
         <v>13</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>40</v>
@@ -2432,40 +2347,65 @@
         <v>8</v>
       </c>
     </row>
+    <row r="59" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J1:P2 J4:P10 J12:P14 J22:P23 J25:P27 J16:P20 J29:P1048576">
-    <cfRule type="expression" dxfId="6" priority="7">
+  <conditionalFormatting sqref="J1:P2 J4:P10 J12:P14 J22:P23 J25:P27 J16:P20 J29:P39 J41:P1048576">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:P3">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>IF(OR($B3="O365Group",$B3="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:P11">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>IF(OR($B11="O365Group",$B11="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:P21">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>IF(OR($B21="O365Group",$B21="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P24">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF(OR($B24="O365Group",$B24="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:P28">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>IF(OR($B28="O365Group",$B28="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:P15">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF(OR($B15="O365Group",$B15="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:P40">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(OR($B15="O365Group",$B15="Type"),faslch,TRUE)</formula>
+      <formula>IF(OR($B40="O365Group",$B40="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2474,18 +2414,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2673,6 +2613,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18209EA7-04F6-445D-8F30-F19FC7D76916}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2684,14 +2632,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merge from customer repos
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0353B1B5-FA76-4349-B814-961782206CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D165C9EC-935C-415A-BD00-409EE9B90799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="2676" windowWidth="21456" windowHeight="12624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7056" yWindow="3192" windowWidth="30960" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="181">
   <si>
     <t>Type</t>
   </si>
@@ -102,9 +102,6 @@
     <t>MFA is enabled for members in this group</t>
   </si>
   <si>
-    <t>Members of this group can register devices</t>
-  </si>
-  <si>
     <t>Holds all devices with a standard configuration</t>
   </si>
   <si>
@@ -565,6 +562,12 @@
   </si>
   <si>
     <t>Holds all users with specified plan assigned</t>
+  </si>
+  <si>
+    <t>Members of this group can register devices and have local admin rights</t>
+  </si>
+  <si>
+    <t>AllowAzureAdRoles</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1139,6 +1144,9 @@
       <c r="P1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1148,10 +1156,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1168,10 +1176,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -1189,13 +1197,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
@@ -1210,13 +1218,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
@@ -1231,13 +1239,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
         <v>152</v>
-      </c>
-      <c r="D6" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" t="s">
-        <v>153</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
@@ -1249,25 +1257,25 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1296,19 +1304,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -1343,25 +1351,25 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
         <v>174</v>
-      </c>
-      <c r="C9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>175</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1385,10 +1393,10 @@
         <v>1</v>
       </c>
       <c r="Q9" t="s">
+        <v>175</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1399,16 +1407,19 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="Q10" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1419,19 +1430,19 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1442,19 +1453,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1465,19 +1476,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1488,19 +1499,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1511,19 +1522,19 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1534,19 +1545,19 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1557,19 +1568,19 @@
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1580,19 +1591,19 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1603,19 +1614,19 @@
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1626,19 +1637,19 @@
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1649,19 +1660,19 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1672,19 +1683,19 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1695,19 +1706,19 @@
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1718,19 +1729,19 @@
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1741,19 +1752,19 @@
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1764,19 +1775,19 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1787,19 +1798,19 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1810,19 +1821,19 @@
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1833,19 +1844,19 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1856,19 +1867,19 @@
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1879,19 +1890,19 @@
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1902,19 +1913,19 @@
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1925,19 +1936,19 @@
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1948,19 +1959,19 @@
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1971,19 +1982,19 @@
         <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1994,19 +2005,19 @@
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2017,19 +2028,19 @@
         <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2040,19 +2051,19 @@
         <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2063,19 +2074,19 @@
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2086,19 +2097,19 @@
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2109,19 +2120,19 @@
         <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2132,19 +2143,19 @@
         <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2155,19 +2166,19 @@
         <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2178,19 +2189,19 @@
         <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2201,19 +2212,19 @@
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2224,19 +2235,19 @@
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2247,19 +2258,19 @@
         <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2270,19 +2281,19 @@
         <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2293,19 +2304,19 @@
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2316,19 +2327,19 @@
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2339,19 +2350,19 @@
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2362,19 +2373,19 @@
         <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2385,19 +2396,19 @@
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2408,19 +2419,19 @@
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2431,19 +2442,19 @@
         <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2454,19 +2465,19 @@
         <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2477,19 +2488,19 @@
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2500,19 +2511,19 @@
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2523,19 +2534,19 @@
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2546,19 +2557,19 @@
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2569,13 +2580,13 @@
         <v>12</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>8</v>
@@ -2589,13 +2600,13 @@
         <v>12</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>8</v>
@@ -2609,13 +2620,13 @@
         <v>12</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>8</v>
@@ -2629,13 +2640,13 @@
         <v>12</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>8</v>
@@ -2649,13 +2660,13 @@
         <v>12</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>8</v>
@@ -2669,13 +2680,13 @@
         <v>12</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>8</v>
@@ -2689,13 +2700,13 @@
         <v>12</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>8</v>
@@ -2709,13 +2720,13 @@
         <v>12</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
New groups and roles
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D165C9EC-935C-415A-BD00-409EE9B90799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC1CCE-3435-4AA0-8D56-4BAE95B4C285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7056" yWindow="3192" windowWidth="30960" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="372" yWindow="348" windowWidth="33456" windowHeight="15528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="182">
   <si>
     <t>Type</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>AllowAzureAdRoles</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -1076,11 +1079,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1095,7 +1096,7 @@
     <col min="9" max="9" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1147,8 +1148,11 @@
       <c r="Q1" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1210,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1231,7 +1235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1346,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1392,14 +1396,14 @@
       <c r="P9" t="b">
         <v>1</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>175</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="S9" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1491,7 +1495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -2799,7 +2803,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="R9" r:id="rId1" xr:uid="{6406F3B4-332F-49FC-A4BF-E9A46FEED504}"/>
+    <hyperlink ref="S9" r:id="rId1" xr:uid="{6406F3B4-332F-49FC-A4BF-E9A46FEED504}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2807,6 +2811,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -2990,12 +3000,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3006,6 +3010,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18209EA7-04F6-445D-8F30-F19FC7D76916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e7596eec-0011-44fa-9047-92dcd650b5d7"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3023,22 +3043,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18209EA7-04F6-445D-8F30-F19FC7D76916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e7596eec-0011-44fa-9047-92dcd650b5d7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Sync with customer repos
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen.xlsx
+++ b/data/aad/Gruppen.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F39EE38-2201-465B-BCF1-5C6915015A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4286C5EF-E9DE-4BD9-8476-758C4A5DF559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5604" yWindow="48" windowWidth="24480" windowHeight="13428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8112" yWindow="1152" windowWidth="28236" windowHeight="14928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gruppen!$A$1:$T$140</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="267">
   <si>
     <t>Type</t>
   </si>
@@ -816,15 +819,6 @@
     <t>ALYASG-LIC-PROJECT3</t>
   </si>
   <si>
-    <t>ALYASG-ADM-KEYAUTHENABLED</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-KEYAUTHENABLEDCLOUD</t>
-  </si>
-  <si>
-    <t>ALYASG-ADM-KEYAUTHENABLEDONPREM</t>
-  </si>
-  <si>
     <t>ParentGroup</t>
   </si>
   <si>
@@ -832,6 +826,9 @@
   </si>
   <si>
     <t>ALYASG-ADM-NOMFADEFAULTS</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PROJECT3ONPREM</t>
   </si>
 </sst>
 </file>
@@ -921,49 +918,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -1108,6 +1063,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>699246</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>116542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1694329</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37F9DC91-3AD1-B774-DFF3-41E595C9BC86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12129246" y="10874189"/>
+          <a:ext cx="995083" cy="1192305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1100"/>
+            <a:t>Remove these licenses, if you use OnPrem</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-CH" sz="1100" baseline="0"/>
+            <a:t> and Cloud license groups</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1431,9 +1466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T138"/>
+  <dimension ref="A1:T140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1501,7 +1538,7 @@
         <v>176</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>177</v>
@@ -1515,13 +1552,13 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -1547,7 +1584,7 @@
         <v>8</v>
       </c>
       <c r="R3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1570,7 +1607,7 @@
         <v>8</v>
       </c>
       <c r="R4" t="s">
-        <v>268</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1593,7 +1630,7 @@
         <v>8</v>
       </c>
       <c r="R5" t="s">
-        <v>268</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1616,6 +1653,7 @@
       <c r="G6" t="s">
         <v>8</v>
       </c>
+      <c r="R6"/>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1637,6 +1675,9 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
+      <c r="R7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1657,6 +1698,9 @@
       <c r="F8"/>
       <c r="G8" t="s">
         <v>8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1667,7 +1711,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D9" t="s">
         <v>257</v>
@@ -1680,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="R9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1691,7 +1735,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D10" t="s">
         <v>258</v>
@@ -1704,7 +1748,7 @@
         <v>8</v>
       </c>
       <c r="R10" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1715,7 +1759,7 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D11" t="s">
         <v>259</v>
@@ -1728,7 +1772,7 @@
         <v>8</v>
       </c>
       <c r="R11" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1751,6 +1795,7 @@
       <c r="G12" t="s">
         <v>8</v>
       </c>
+      <c r="R12"/>
     </row>
     <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1772,6 +1817,7 @@
       <c r="G13" t="s">
         <v>8</v>
       </c>
+      <c r="R13"/>
     </row>
     <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1793,6 +1839,7 @@
       <c r="G14" t="s">
         <v>8</v>
       </c>
+      <c r="R14"/>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1814,6 +1861,9 @@
       <c r="G15" t="s">
         <v>8</v>
       </c>
+      <c r="R15" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1834,6 +1884,9 @@
       <c r="F16"/>
       <c r="G16" t="s">
         <v>8</v>
+      </c>
+      <c r="R16" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
@@ -3371,6 +3424,9 @@
       <c r="I79" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="R79" s="6" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="80" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
@@ -3394,6 +3450,9 @@
       <c r="I80" s="6" t="s">
         <v>159</v>
       </c>
+      <c r="R80" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="81" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
@@ -3417,6 +3476,9 @@
       <c r="I81" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="R81" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="82" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
@@ -3440,6 +3502,9 @@
       <c r="I82" s="6" t="s">
         <v>201</v>
       </c>
+      <c r="R82" s="6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="83" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
@@ -3463,6 +3528,9 @@
       <c r="I83" s="6" t="s">
         <v>200</v>
       </c>
+      <c r="R83" s="6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="84" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
@@ -3486,6 +3554,9 @@
       <c r="I84" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="R84" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="85" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
@@ -3510,7 +3581,7 @@
         <v>84</v>
       </c>
       <c r="R85" s="6" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3535,6 +3606,9 @@
       <c r="I86" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="R86" s="6" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="87" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
@@ -3558,6 +3632,9 @@
       <c r="I87" s="6" t="s">
         <v>85</v>
       </c>
+      <c r="R87" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="88" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
@@ -3581,6 +3658,9 @@
       <c r="I88" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="R88" s="6" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="89" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
@@ -3604,6 +3684,9 @@
       <c r="I89" s="6" t="s">
         <v>86</v>
       </c>
+      <c r="R89" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="90" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
@@ -3627,6 +3710,9 @@
       <c r="I90" s="6" t="s">
         <v>87</v>
       </c>
+      <c r="R90" s="6" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="91" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
@@ -3650,6 +3736,9 @@
       <c r="I91" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="R91" s="6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="92" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
@@ -3674,7 +3763,7 @@
         <v>145</v>
       </c>
       <c r="R92" s="6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3700,7 +3789,7 @@
         <v>88</v>
       </c>
       <c r="R93" s="6" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3726,7 +3815,7 @@
         <v>43</v>
       </c>
       <c r="R94" s="6" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3751,6 +3840,9 @@
       <c r="I95" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="R95" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="96" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
@@ -3774,6 +3866,9 @@
       <c r="I96" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="R96" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="97" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
@@ -3797,6 +3892,9 @@
       <c r="I97" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="R97" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="98" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
@@ -3820,6 +3918,9 @@
       <c r="I98" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="R98" s="6" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="99" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
@@ -3843,6 +3944,9 @@
       <c r="I99" s="6" t="s">
         <v>90</v>
       </c>
+      <c r="R99" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="100" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
@@ -3866,6 +3970,9 @@
       <c r="I100" s="6" t="s">
         <v>91</v>
       </c>
+      <c r="R100" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="101" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
@@ -3889,6 +3996,9 @@
       <c r="I101" s="6" t="s">
         <v>92</v>
       </c>
+      <c r="R101" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="102" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
@@ -3912,6 +4022,9 @@
       <c r="I102" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="R102" s="6" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="103" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
@@ -3921,10 +4034,10 @@
         <v>190</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>31</v>
@@ -3933,7 +4046,10 @@
         <v>8</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>93</v>
+        <v>261</v>
+      </c>
+      <c r="R103" s="6" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3944,42 +4060,48 @@
         <v>190</v>
       </c>
       <c r="C104" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="R104" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C105" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D104" s="6" t="s">
+      <c r="D105" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I104" s="6" t="s">
+      <c r="E105" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" s="6" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>81</v>
+      <c r="R105" s="6" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3990,10 +4112,10 @@
         <v>12</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>31</v>
@@ -4002,7 +4124,10 @@
         <v>8</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>159</v>
+        <v>81</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4013,10 +4138,10 @@
         <v>12</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>31</v>
@@ -4025,7 +4150,10 @@
         <v>8</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>82</v>
+        <v>159</v>
+      </c>
+      <c r="R107" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4036,10 +4164,10 @@
         <v>12</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>31</v>
@@ -4048,7 +4176,10 @@
         <v>8</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>201</v>
+        <v>82</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4059,10 +4190,10 @@
         <v>12</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>31</v>
@@ -4071,7 +4202,10 @@
         <v>8</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="R109" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4082,10 +4216,10 @@
         <v>12</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>31</v>
@@ -4094,7 +4228,10 @@
         <v>8</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>83</v>
+        <v>200</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="111" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4105,10 +4242,10 @@
         <v>12</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>31</v>
@@ -4117,10 +4254,10 @@
         <v>8</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R111" s="3" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4131,10 +4268,10 @@
         <v>12</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>31</v>
@@ -4143,7 +4280,10 @@
         <v>8</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>33</v>
+        <v>84</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4154,10 +4294,10 @@
         <v>12</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>31</v>
@@ -4166,7 +4306,10 @@
         <v>8</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>85</v>
+        <v>33</v>
+      </c>
+      <c r="R113" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4177,10 +4320,10 @@
         <v>12</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>31</v>
@@ -4189,7 +4332,10 @@
         <v>8</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>35</v>
+        <v>85</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4200,10 +4346,10 @@
         <v>12</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>31</v>
@@ -4212,7 +4358,10 @@
         <v>8</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>86</v>
+        <v>35</v>
+      </c>
+      <c r="R115" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="116" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4223,10 +4372,10 @@
         <v>12</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>31</v>
@@ -4235,7 +4384,10 @@
         <v>8</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4246,10 +4398,10 @@
         <v>12</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>31</v>
@@ -4258,7 +4410,10 @@
         <v>8</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>42</v>
+        <v>87</v>
+      </c>
+      <c r="R117" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="118" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4269,10 +4424,10 @@
         <v>12</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>31</v>
@@ -4281,10 +4436,10 @@
         <v>8</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="R118" s="3" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="119" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4295,10 +4450,10 @@
         <v>12</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>31</v>
@@ -4307,10 +4462,10 @@
         <v>8</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="R119" s="3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4321,10 +4476,10 @@
         <v>12</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>31</v>
@@ -4333,10 +4488,10 @@
         <v>8</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="R120" s="3" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4347,10 +4502,10 @@
         <v>12</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>31</v>
@@ -4359,7 +4514,10 @@
         <v>8</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="R121" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="122" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4370,10 +4528,10 @@
         <v>12</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>31</v>
@@ -4382,7 +4540,10 @@
         <v>8</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>89</v>
+        <v>32</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="123" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4393,10 +4554,10 @@
         <v>12</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>31</v>
@@ -4405,7 +4566,10 @@
         <v>8</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>34</v>
+        <v>89</v>
+      </c>
+      <c r="R123" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4416,10 +4580,10 @@
         <v>12</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>31</v>
@@ -4428,7 +4592,10 @@
         <v>8</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4439,10 +4606,10 @@
         <v>12</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>31</v>
@@ -4451,7 +4618,10 @@
         <v>8</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>90</v>
+        <v>45</v>
+      </c>
+      <c r="R125" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4462,10 +4632,10 @@
         <v>12</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>31</v>
@@ -4474,7 +4644,10 @@
         <v>8</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4485,10 +4658,10 @@
         <v>12</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>31</v>
@@ -4497,7 +4670,10 @@
         <v>8</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="R127" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4508,119 +4684,140 @@
         <v>12</v>
       </c>
       <c r="C128" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D129" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E128" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I128" s="3" t="s">
+      <c r="E129" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="R129" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D131" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E129" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I129" s="3" t="s">
+      <c r="E131" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" s="3" t="s">
+      <c r="R131" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D132" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E130" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I130" s="3" t="s">
+      <c r="E132" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="3" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C131" s="4" t="s">
+      <c r="R132" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D133" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E131" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G131" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D132" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E132" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G132" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>36</v>
@@ -4629,7 +4826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>23</v>
       </c>
@@ -4637,10 +4834,10 @@
         <v>12</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>36</v>
@@ -4649,7 +4846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>23</v>
       </c>
@@ -4657,50 +4854,50 @@
         <v>12</v>
       </c>
       <c r="C135" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D137" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="E135" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G135" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E136" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G136" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D137" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>37</v>
@@ -4709,7 +4906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>23</v>
       </c>
@@ -4717,10 +4914,10 @@
         <v>12</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>37</v>
@@ -4729,130 +4926,141 @@
         <v>8</v>
       </c>
     </row>
+    <row r="139" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G139" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G140" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J29:P31 J39:P40 J42:P44 J33:P37 J52:P52 J54:P55 J57:P64 J26:P27 J14:P18 J20:P23 J66:P75 J81:P82 J84:P91 J93:P105 J107:P108 J110:P117 J1:P1 J77:P79 J119:P1048576 J3:P11">
-    <cfRule type="expression" dxfId="24" priority="27">
+  <autoFilter ref="A1:T140" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="J52:P52 J54:P55 J57:P64 J14:P18 J66:P75 J81:P82 J84:P91 J93:P102 J108:P109 J111:P118 J1:P1 J77:P79 J3:P11 J104:P106 J120:P129 J131:P1048576">
+    <cfRule type="expression" dxfId="18" priority="32">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:P13">
-    <cfRule type="expression" dxfId="23" priority="26">
+    <cfRule type="expression" dxfId="17" priority="31">
       <formula>IF(OR($B12="O365Group",$B12="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:P28">
-    <cfRule type="expression" dxfId="22" priority="25">
-      <formula>IF(OR($B28="O365Group",$B28="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38:P38">
-    <cfRule type="expression" dxfId="21" priority="24">
-      <formula>IF(OR($B38="O365Group",$B38="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:P41">
-    <cfRule type="expression" dxfId="20" priority="23">
-      <formula>IF(OR($B41="O365Group",$B41="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45:P45">
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>IF(OR($B45="O365Group",$B45="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32:P32">
-    <cfRule type="expression" dxfId="18" priority="21">
-      <formula>IF(OR($B32="O365Group",$B32="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J65:P65">
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="16" priority="25">
       <formula>IF(OR($B65="O365Group",$B65="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47:P47 J50:P51">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>IF(OR($B47="O365Group",$B47="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:P46">
-    <cfRule type="expression" dxfId="15" priority="18">
-      <formula>IF(OR($B46="O365Group",$B46="Type"),faslch,TRUE)</formula>
+  <conditionalFormatting sqref="J50:P51">
+    <cfRule type="expression" dxfId="15" priority="24">
+      <formula>IF(OR($B50="O365Group",$B50="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53:P53">
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="14" priority="22">
       <formula>IF(OR($B53="O365Group",$B53="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:P56">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="13" priority="21">
       <formula>IF(OR($B56="O365Group",$B56="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:P19">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>IF(OR($B19="O365Group",$B19="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:P24">
-    <cfRule type="expression" dxfId="11" priority="14">
-      <formula>IF(OR($B24="O365Group",$B24="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25:P25">
-    <cfRule type="expression" dxfId="10" priority="13">
-      <formula>IF(OR($B25="O365Group",$B25="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J48:P48">
-    <cfRule type="expression" dxfId="9" priority="12">
-      <formula>IF(OR($B48="O365Group",$B48="Type"),faslch,TRUE)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J49:P49">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="11" priority="16">
       <formula>IF(OR($B49="O365Group",$B49="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:P92">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>IF(OR($B92="O365Group",$B92="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:P80">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>IF(OR($B80="O365Group",$B80="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:P83">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>IF(OR($B83="O365Group",$B83="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J118:P118">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>IF(OR($B118="O365Group",$B118="Type"),faslch,TRUE)</formula>
+  <conditionalFormatting sqref="J119:P119">
+    <cfRule type="expression" dxfId="7" priority="10">
+      <formula>IF(OR($B119="O365Group",$B119="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J106:P106">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>IF(OR($B106="O365Group",$B106="Type"),faslch,TRUE)</formula>
+  <conditionalFormatting sqref="J107:P107">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>IF(OR($B107="O365Group",$B107="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J109:P109">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>IF(OR($B109="O365Group",$B109="Type"),faslch,TRUE)</formula>
+  <conditionalFormatting sqref="J110:P110">
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>IF(OR($B110="O365Group",$B110="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:P76">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>IF(OR($B76="O365Group",$B76="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:P2">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>IF(OR($B2="O365Group",$B2="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J103:P103">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>IF(OR($B103="O365Group",$B103="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J130:P130">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF(OR($B130="O365Group",$B130="Type"),faslch,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:P48">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(OR($B2="O365Group",$B2="Type"),faslch,TRUE)</formula>
+      <formula>IF(OR($B20="O365Group",$B20="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -4860,6 +5068,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>